<commit_message>
Script to calculate TGT resistor added.
</commit_message>
<xml_diff>
--- a/data/instrument_characteristics.xlsx
+++ b/data/instrument_characteristics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dougal/src/TBAG/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02399746-4B11-4246-9A93-413CED14E446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F66279F-11BB-1845-B089-F33D79DAAA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{E67E785D-E7DA-4C45-B70F-B9A10FD1447D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Instrument</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Resistor with 5V supply to work</t>
+  </si>
+  <si>
+    <t>9.27 k Ohms with 541 Ohm dampener</t>
   </si>
 </sst>
 </file>
@@ -448,15 +451,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E09828-E540-284E-A40D-75FD5E660353}">
-  <dimension ref="A7:G9"/>
+  <dimension ref="A7:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,7 +479,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -496,7 +499,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -514,6 +517,9 @@
       </c>
       <c r="G9" t="s">
         <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Engine warning lights added.
</commit_message>
<xml_diff>
--- a/data/instrument_characteristics.xlsx
+++ b/data/instrument_characteristics.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dougal/src/TBAG/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F66279F-11BB-1845-B089-F33D79DAAA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD20300B-5E91-9440-93DB-F3DB85A38D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{E67E785D-E7DA-4C45-B70F-B9A10FD1447D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -90,7 +91,7 @@
     <t>Resistor with 5V supply to work</t>
   </si>
   <si>
-    <t>9.27 k Ohms with 541 Ohm dampener</t>
+    <t>5.6 k Ohms with 56 Ohm dampener</t>
   </si>
 </sst>
 </file>
@@ -525,4 +526,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD43E307-2EB8-844A-910D-EE18921E5E31}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>